<commit_message>
added MalaCard gene tsv files
</commit_message>
<xml_diff>
--- a/Data/ChenGenes_MalaCards.xlsx
+++ b/Data/ChenGenes_MalaCards.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10113"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Accounts/chens5/Desktop/CompBioComps/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katefinstuen-magro/Desktop/comps/CompBioComps/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50AECB5B-BA59-F846-A2E6-BC0A78341619}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2820" yWindow="1900" windowWidth="29700" windowHeight="18280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="460" yWindow="1140" windowWidth="28800" windowHeight="16500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Ischaemic stroke" sheetId="1" r:id="rId1"/>
     <sheet name="Endometriosis" sheetId="2" r:id="rId2"/>
     <sheet name="Lymphoma" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150000"/>
+  <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -1187,7 +1186,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1504,11 +1503,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="97" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="97" workbookViewId="0">
+      <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2458,7 +2457,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K44"/>
   <sheetViews>
     <sheetView topLeftCell="A11" workbookViewId="0">
@@ -3240,7 +3239,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L43"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>